<commit_message>
Added pull vol script; added old update script; changed path to final output files
</commit_message>
<xml_diff>
--- a/exception_list.xlsx
+++ b/exception_list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="11730"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="11730" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="bandit" sheetId="1" r:id="rId1"/>
@@ -377,7 +377,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -440,10 +440,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,6 +476,31 @@
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>218219</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>213163</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>221080</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>221099</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>202278</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>221183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added scheduler and minor tweaks due to database woes
</commit_message>
<xml_diff>
--- a/exception_list.xlsx
+++ b/exception_list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="11730" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="11730" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="bandit" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="clockbpd" sheetId="5" r:id="rId5"/>
     <sheet name="trust_bpd" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -375,10 +375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,6 +433,11 @@
         <v>220740</v>
       </c>
     </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>220989</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -442,7 +447,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D22" sqref="D22:D23"/>
     </sheetView>
   </sheetViews>
@@ -522,10 +527,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,6 +543,16 @@
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>216806</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>219944</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>37542</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lastest changes before departure, adding execption subjs, new tasks, README updates
</commit_message>
<xml_diff>
--- a/exception_list.xlsx
+++ b/exception_list.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\kod\automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="11730" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="11730" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="bandit" sheetId="1" r:id="rId1"/>
@@ -445,10 +445,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22:D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,6 +506,26 @@
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>221183</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>214082</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>220889</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>220989</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>221085</v>
       </c>
     </row>
   </sheetData>
@@ -529,7 +549,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>

</xml_diff>